<commit_message>
Gentable  & Workflow vsd updates
</commit_message>
<xml_diff>
--- a/DbLayouts/XX-系統/TxToDoMain.xlsx
+++ b/DbLayouts/XX-系統/TxToDoMain.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="225">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1115,10 +1115,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>銀扣失敗書面通知單</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>L4454</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1148,6 +1144,22 @@
   </si>
   <si>
     <t>C-連結處理交易，交易處理後由TxToDoCom共用程式將明細檔狀態更改為已處理</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>L4454</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTI02</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>銀扣失敗繳息還本通知單</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>銀扣二扣失敗明信片</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -1309,7 +1321,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1453,6 +1465,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2371,10 +2386,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2393,7 +2408,7 @@
         <v>76</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C1" s="47" t="s">
         <v>71</v>
@@ -3535,7 +3550,7 @@
         <v>212</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C32" s="39" t="s">
         <v>119</v>
@@ -3562,76 +3577,114 @@
         <v>119</v>
       </c>
       <c r="K32" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="L32" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="L32" s="45" t="s">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" s="39" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="39" t="s">
+      <c r="C33" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="J33" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="L33" s="45" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="39" t="s">
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="48"/>
+      <c r="C36" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="39"/>
-      <c r="C35" s="39" t="s">
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="48"/>
+      <c r="C37" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="48"/>
+      <c r="C38" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="39"/>
-      <c r="C36" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="39"/>
-      <c r="C37" s="39" t="s">
-        <v>220</v>
-      </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>